<commit_message>
updated scripts for cph schools
</commit_message>
<xml_diff>
--- a/data_prep/SummaryTable.xlsx
+++ b/data_prep/SummaryTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CPH_data_summary" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="209">
   <si>
     <t>Type</t>
   </si>
@@ -699,17 +699,35 @@
     <t>http://wms.pcn.minambiente.it/ogc?map=/ms_ogc/wfs/RAMSAR.map&amp;Service=WFS</t>
   </si>
   <si>
-    <t>Administrative</t>
-  </si>
-  <si>
-    <t>https://www.istat.it/it/archivio/104317</t>
+    <t>https://inspire-geoportal.ec.europa.eu/download_details.html?view=downloadDetails&amp;resourceId=%2FINSPIRE-8c93a17a-05f4-11e1-b7de-52540004b857_20210601-160602%2Fservices%2F1%2FPullResults%2F21-40%2Fdatasets%2F12&amp;expandedSection=download</t>
+  </si>
+  <si>
+    <t>INSPIRE</t>
+  </si>
+  <si>
+    <t>gpkg</t>
+  </si>
+  <si>
+    <t>Home Value</t>
+  </si>
+  <si>
+    <t>Sales Prices per m2</t>
+  </si>
+  <si>
+    <t>https://maps.amsterdam.nl/woningwaarde/ &gt;</t>
+  </si>
+  <si>
+    <t>Maps Amsterdam</t>
+  </si>
+  <si>
+    <t>shp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +773,14 @@
       <color rgb="FF323232"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -943,10 +969,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1070,8 +1097,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1352,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="E22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37:L37"/>
+    <sheetView topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3096,16 +3125,251 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="23.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
+      </c>
+      <c r="H13" t="s">
+        <v>208</v>
+      </c>
+      <c r="I13" t="s">
+        <v>207</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="M13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A13:B15"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A5:B9"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="C8:C9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J13" r:id="rId1" display="https://maps.amsterdam.nl/woningwaarde/?LANG=nl"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
@@ -3145,7 +3409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="207" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>34</v>
       </c>
@@ -3155,10 +3419,10 @@
         <v>35</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>29</v>
@@ -3177,11 +3441,6 @@
       </c>
       <c r="L2" s="17" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3192,349 +3451,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="207" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A13:B17"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:B12"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3958,14 +3880,6 @@
       </c>
       <c r="L26" s="9" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>201</v>
-      </c>
-      <c r="M28" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new scripts for deliverables
</commit_message>
<xml_diff>
--- a/data_prep/SummaryTable.xlsx
+++ b/data_prep/SummaryTable.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1437B8-D46D-4D90-9141-BC272B8473AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2172" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPH_data_summary" sheetId="1" r:id="rId1"/>
@@ -13,10 +14,19 @@
     <sheet name="ROM_data_summary" sheetId="5" r:id="rId4"/>
     <sheet name="Definitions" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -733,15 +743,6 @@
   </si>
   <si>
     <t>Forests semi natural areas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For the calculation of the avergae housing price per m2, 7 building types were used (# 120: Detached single-family house (detached house).
-# 121: Attached single-family house.
-# 122: Detached single-family house in dense-low-rise area.
-# 130: Townhouse, chain, or semi-detached house (vertical separation between the units).
-# 131: Row and cluster housing.
-# 132: Semi-detached house (double house). 
-# 140: Multi-storey residential building (multi-family house, including two-family house (horizontal separation between the units), selecting additionally the residential buildings that were traded on the ordinary free trade (OVERDRAGELSES_KODE = 1 - Almindelig frit salg) or public sales (OVERDRAGELSES_KODE = 3 - Auktion), since these values represent what people are willing to pay for own a property. </t>
   </si>
   <si>
     <t>2002-2020</t>
@@ -1371,11 +1372,20 @@
   <si>
     <t>2009, 2011, 2015, 2016, 2017, 2018</t>
   </si>
+  <si>
+    <t xml:space="preserve">For the calculation of the average housing price per m2, 7 building types were used (# 120: Detached single-family house (detached house).
+# 121: Attached single-family house.
+# 122: Detached single-family house in dense-low-rise area.
+# 130: Townhouse, chain, or semi-detached house (vertical separation between the units).
+# 131: Row and cluster housing.
+# 132: Semi-detached house (double house). 
+# 140: Multi-storey residential building (multi-family house, including two-family house (horizontal separation between the units), selecting additionally the residential buildings that were traded on the ordinary free trade (OVERDRAGELSES_KODE = 1 - Almindelig frit salg) or public sales (OVERDRAGELSES_KODE = 3 - Auktion), since these values represent what people are willing to pay for own a property. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1716,7 +1726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1998,6 +2008,9 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2278,11 +2291,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2338,7 +2351,7 @@
         <v>22</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>0</v>
@@ -2504,7 +2517,7 @@
         <v>23</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2539,7 +2552,7 @@
         <v>23</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2572,7 +2585,7 @@
         <v>23</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2605,7 +2618,7 @@
         <v>23</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q9" s="51" t="s">
         <v>158</v>
@@ -2641,7 +2654,7 @@
         <v>23</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q10" s="51" t="s">
         <v>157</v>
@@ -2677,10 +2690,10 @@
         <v>23</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q11" s="51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2715,7 +2728,7 @@
         <v>23</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q12" s="51"/>
     </row>
@@ -2749,7 +2762,7 @@
         <v>23</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2782,7 +2795,7 @@
         <v>23</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2815,7 +2828,7 @@
         <v>23</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
@@ -2852,7 +2865,7 @@
         <v>23</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O16" s="7"/>
     </row>
@@ -2890,7 +2903,7 @@
         <v>23</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O17" s="7"/>
     </row>
@@ -2928,7 +2941,7 @@
         <v>23</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O18" s="7"/>
     </row>
@@ -2962,7 +2975,7 @@
         <v>23</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="O19" s="7"/>
     </row>
@@ -3000,7 +3013,7 @@
         <v>23</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3033,7 +3046,7 @@
         <v>23</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3066,7 +3079,7 @@
         <v>23</v>
       </c>
       <c r="M22" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3099,7 +3112,7 @@
         <v>23</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3132,7 +3145,7 @@
         <v>23</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3165,7 +3178,7 @@
         <v>23</v>
       </c>
       <c r="M25" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3202,7 +3215,7 @@
         <v>23</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3239,7 +3252,7 @@
         <v>23</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3272,7 +3285,7 @@
         <v>23</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3309,7 +3322,7 @@
         <v>23</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3342,7 +3355,7 @@
         <v>23</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3377,7 +3390,7 @@
         <v>23</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
@@ -3410,7 +3423,7 @@
         <v>23</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3445,7 +3458,7 @@
         <v>23</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3478,7 +3491,7 @@
         <v>23</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3511,7 +3524,7 @@
         <v>23</v>
       </c>
       <c r="M35" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3550,7 +3563,7 @@
         <v>24</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3587,7 +3600,7 @@
         <v>24</v>
       </c>
       <c r="M37" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3622,7 +3635,7 @@
         <v>24</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3659,7 +3672,7 @@
         <v>24</v>
       </c>
       <c r="M39" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3696,7 +3709,7 @@
         <v>24</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -3733,7 +3746,7 @@
         <v>24</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3867,7 +3880,7 @@
         <v>24</v>
       </c>
       <c r="M45" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -3934,7 +3947,7 @@
         <v>24</v>
       </c>
       <c r="M47" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4033,7 +4046,7 @@
         <v>24</v>
       </c>
       <c r="M50" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -4066,7 +4079,7 @@
         <v>24</v>
       </c>
       <c r="M51" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -4174,10 +4187,10 @@
       <c r="B55" s="75"/>
       <c r="C55" s="77"/>
       <c r="D55" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>25</v>
@@ -4189,19 +4202,19 @@
         <v>39</v>
       </c>
       <c r="I55" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J55" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="K55" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L55" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="J55" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="K55" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="L55" s="52" t="s">
-        <v>217</v>
-      </c>
       <c r="M55" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
@@ -4212,7 +4225,7 @@
         <v>152</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>25</v>
@@ -4224,30 +4237,30 @@
         <v>39</v>
       </c>
       <c r="I56" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J56" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="K56" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L56" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="J56" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="K56" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="L56" s="52" t="s">
-        <v>217</v>
-      </c>
       <c r="M56" s="22" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="220.8" x14ac:dyDescent="0.3">
       <c r="A57" s="74"/>
       <c r="B57" s="75"/>
       <c r="C57" s="80"/>
       <c r="D57" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E57" s="9" t="s">
-        <v>213</v>
+      <c r="E57" s="115" t="s">
+        <v>387</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>25</v>
@@ -4259,19 +4272,19 @@
         <v>39</v>
       </c>
       <c r="I57" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J57" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L57" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="J57" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="L57" s="52" t="s">
-        <v>217</v>
-      </c>
       <c r="M57" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -4384,18 +4397,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="8.88671875" style="15"/>
     <col min="4" max="4" width="18.77734375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" style="15" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" style="15" customWidth="1"/>
     <col min="7" max="7" width="13.77734375" style="15" customWidth="1"/>
     <col min="8" max="8" width="7.5546875" style="15" customWidth="1"/>
@@ -4447,7 +4460,7 @@
         <v>22</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>0</v>
@@ -4489,7 +4502,7 @@
       </c>
       <c r="M2" s="34"/>
       <c r="N2" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O2" s="33"/>
       <c r="P2" s="33"/>
@@ -4500,10 +4513,10 @@
       <c r="B3" s="102"/>
       <c r="C3" s="103"/>
       <c r="D3" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>182</v>
@@ -4513,10 +4526,10 @@
         <v>35</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K3" s="23" t="s">
         <v>127</v>
@@ -4526,7 +4539,7 @@
       </c>
       <c r="M3" s="34"/>
       <c r="N3" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
@@ -4537,10 +4550,10 @@
       <c r="B4" s="102"/>
       <c r="C4" s="103"/>
       <c r="D4" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>182</v>
@@ -4550,10 +4563,10 @@
         <v>35</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>127</v>
@@ -4563,7 +4576,7 @@
       </c>
       <c r="M4" s="34"/>
       <c r="N4" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O4" s="33"/>
       <c r="P4" s="33"/>
@@ -4574,10 +4587,10 @@
       <c r="B5" s="105"/>
       <c r="C5" s="106"/>
       <c r="D5" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>182</v>
@@ -4587,10 +4600,10 @@
         <v>35</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>127</v>
@@ -4600,7 +4613,7 @@
       </c>
       <c r="M5" s="34"/>
       <c r="N5" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
@@ -4614,7 +4627,7 @@
       <c r="C6" s="94"/>
       <c r="D6" s="94"/>
       <c r="E6" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -4627,7 +4640,7 @@
       <c r="N6" s="34"/>
       <c r="O6" s="33"/>
       <c r="P6" s="39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="33"/>
     </row>
@@ -4639,7 +4652,7 @@
       <c r="C7" s="94"/>
       <c r="D7" s="94"/>
       <c r="E7" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -4652,7 +4665,7 @@
       <c r="N7" s="34"/>
       <c r="O7" s="33"/>
       <c r="P7" s="39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q7" s="33"/>
     </row>
@@ -4694,7 +4707,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>28</v>
@@ -4703,22 +4716,22 @@
         <v>39</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J9" s="34"/>
       <c r="K9" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L9" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N9" s="34"/>
       <c r="O9" s="33"/>
       <c r="P9" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q9" s="33"/>
     </row>
@@ -4730,10 +4743,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G10" s="22" t="s">
         <v>28</v>
@@ -4742,17 +4755,17 @@
         <v>39</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J10" s="34"/>
       <c r="K10" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L10" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N10" s="34"/>
       <c r="O10" s="33"/>
@@ -4765,10 +4778,10 @@
       <c r="C11" s="94"/>
       <c r="D11" s="94"/>
       <c r="E11" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="22" t="s">
         <v>28</v>
@@ -4777,17 +4790,17 @@
         <v>39</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J11" s="34"/>
       <c r="K11" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L11" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="33"/>
@@ -4800,10 +4813,10 @@
       <c r="C12" s="94"/>
       <c r="D12" s="94"/>
       <c r="E12" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>28</v>
@@ -4812,17 +4825,17 @@
         <v>39</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J12" s="34"/>
       <c r="K12" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="33"/>
@@ -4835,10 +4848,10 @@
       <c r="C13" s="94"/>
       <c r="D13" s="94"/>
       <c r="E13" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>28</v>
@@ -4847,17 +4860,17 @@
         <v>39</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J13" s="34"/>
       <c r="K13" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L13" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="33"/>
@@ -4870,10 +4883,10 @@
       <c r="C14" s="94"/>
       <c r="D14" s="94"/>
       <c r="E14" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>28</v>
@@ -4882,17 +4895,17 @@
         <v>39</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L14" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N14" s="34"/>
       <c r="O14" s="33"/>
@@ -4907,10 +4920,10 @@
         <v>19</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>28</v>
@@ -4919,17 +4932,17 @@
         <v>39</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N15" s="34"/>
       <c r="O15" s="33"/>
@@ -4942,10 +4955,10 @@
       <c r="C16" s="94"/>
       <c r="D16" s="94"/>
       <c r="E16" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>28</v>
@@ -4954,17 +4967,17 @@
         <v>39</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N16" s="34"/>
       <c r="O16" s="33"/>
@@ -4977,10 +4990,10 @@
       <c r="C17" s="94"/>
       <c r="D17" s="94"/>
       <c r="E17" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>28</v>
@@ -4989,17 +5002,17 @@
         <v>39</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L17" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N17" s="34"/>
       <c r="O17" s="33"/>
@@ -5015,7 +5028,7 @@
         <v>68</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>28</v>
@@ -5024,17 +5037,17 @@
         <v>39</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J18" s="34"/>
       <c r="K18" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L18" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N18" s="34"/>
       <c r="O18" s="33"/>
@@ -5054,7 +5067,7 @@
         <v>72</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>28</v>
@@ -5063,17 +5076,17 @@
         <v>39</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J19" s="34"/>
       <c r="K19" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L19" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N19" s="34"/>
       <c r="O19" s="33"/>
@@ -5093,7 +5106,7 @@
         <v>75</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>28</v>
@@ -5102,17 +5115,17 @@
         <v>39</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J20" s="34"/>
       <c r="K20" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L20" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N20" s="34"/>
       <c r="O20" s="33"/>
@@ -5172,7 +5185,7 @@
         <v>83</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>28</v>
@@ -5181,17 +5194,17 @@
         <v>39</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J23" s="34"/>
       <c r="K23" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L23" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N23" s="34"/>
       <c r="O23" s="33"/>
@@ -5207,7 +5220,7 @@
         <v>85</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G24" s="22" t="s">
         <v>28</v>
@@ -5216,17 +5229,17 @@
         <v>39</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J24" s="34"/>
       <c r="K24" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L24" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N24" s="34"/>
       <c r="O24" s="33"/>
@@ -5242,7 +5255,7 @@
         <v>87</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>28</v>
@@ -5251,17 +5264,17 @@
         <v>39</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J25" s="34"/>
       <c r="K25" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L25" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M25" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N25" s="34"/>
       <c r="O25" s="33"/>
@@ -5274,10 +5287,10 @@
       <c r="C26" s="97"/>
       <c r="D26" s="97"/>
       <c r="E26" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>28</v>
@@ -5286,17 +5299,17 @@
         <v>39</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J26" s="34"/>
       <c r="K26" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L26" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N26" s="34"/>
       <c r="O26" s="33"/>
@@ -5309,10 +5322,10 @@
       <c r="C27" s="97"/>
       <c r="D27" s="97"/>
       <c r="E27" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>28</v>
@@ -5321,17 +5334,17 @@
         <v>39</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J27" s="34"/>
       <c r="K27" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L27" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N27" s="34"/>
       <c r="O27" s="33"/>
@@ -5344,10 +5357,10 @@
       <c r="C28" s="97"/>
       <c r="D28" s="97"/>
       <c r="E28" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>28</v>
@@ -5356,17 +5369,17 @@
         <v>39</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J28" s="34"/>
       <c r="K28" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L28" s="22" t="s">
         <v>23</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N28" s="34"/>
       <c r="O28" s="33"/>
@@ -5383,29 +5396,29 @@
         <v>20</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I29" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I29" s="22" t="s">
-        <v>271</v>
-      </c>
       <c r="J29" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L29" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N29" s="34"/>
       <c r="O29" s="33"/>
@@ -5418,29 +5431,29 @@
       <c r="C30" s="97"/>
       <c r="D30" s="97"/>
       <c r="E30" s="29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G30" s="22"/>
       <c r="H30" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I30" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I30" s="22" t="s">
-        <v>271</v>
-      </c>
       <c r="J30" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K30" s="27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L30" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N30" s="34"/>
       <c r="O30" s="33"/>
@@ -5453,29 +5466,29 @@
       <c r="C31" s="97"/>
       <c r="D31" s="97"/>
       <c r="E31" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G31" s="22"/>
       <c r="H31" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I31" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="I31" s="22" t="s">
-        <v>271</v>
-      </c>
       <c r="J31" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K31" s="27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L31" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N31" s="34"/>
       <c r="O31" s="33"/>
@@ -5489,30 +5502,30 @@
         <v>21</v>
       </c>
       <c r="D32" s="97" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I32" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J32" s="34"/>
       <c r="K32" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L32" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N32" s="34"/>
       <c r="O32" s="33"/>
@@ -5525,27 +5538,27 @@
       <c r="C33" s="108"/>
       <c r="D33" s="97"/>
       <c r="E33" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I33" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I33" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J33" s="34"/>
       <c r="K33" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L33" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N33" s="34"/>
       <c r="O33" s="33"/>
@@ -5558,27 +5571,27 @@
       <c r="C34" s="108"/>
       <c r="D34" s="97"/>
       <c r="E34" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I34" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I34" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J34" s="34"/>
       <c r="K34" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L34" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N34" s="34"/>
       <c r="O34" s="33"/>
@@ -5591,27 +5604,27 @@
       <c r="C35" s="108"/>
       <c r="D35" s="97"/>
       <c r="E35" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I35" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J35" s="34"/>
       <c r="K35" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L35" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M35" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N35" s="34"/>
       <c r="O35" s="33"/>
@@ -5624,27 +5637,27 @@
       <c r="C36" s="108"/>
       <c r="D36" s="97"/>
       <c r="E36" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I36" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I36" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J36" s="34"/>
       <c r="K36" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L36" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M36" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N36" s="34"/>
       <c r="O36" s="33"/>
@@ -5657,27 +5670,27 @@
       <c r="C37" s="108"/>
       <c r="D37" s="97"/>
       <c r="E37" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I37" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J37" s="34"/>
       <c r="K37" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L37" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M37" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N37" s="34"/>
       <c r="O37" s="33"/>
@@ -5689,30 +5702,30 @@
       <c r="B38" s="94"/>
       <c r="C38" s="108"/>
       <c r="D38" s="97" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I38" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J38" s="34"/>
       <c r="K38" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L38" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N38" s="34"/>
       <c r="O38" s="33"/>
@@ -5725,27 +5738,27 @@
       <c r="C39" s="108"/>
       <c r="D39" s="97"/>
       <c r="E39" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I39" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I39" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J39" s="34"/>
       <c r="K39" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L39" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M39" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N39" s="34"/>
       <c r="O39" s="33"/>
@@ -5758,27 +5771,27 @@
       <c r="C40" s="108"/>
       <c r="D40" s="97"/>
       <c r="E40" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I40" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I40" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J40" s="34"/>
       <c r="K40" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L40" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N40" s="34"/>
       <c r="O40" s="33"/>
@@ -5791,32 +5804,32 @@
       <c r="C41" s="109"/>
       <c r="D41" s="97"/>
       <c r="E41" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G41" s="22"/>
       <c r="H41" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="I41" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="J41" s="34"/>
       <c r="K41" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L41" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N41" s="34"/>
       <c r="O41" s="33"/>
       <c r="P41" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q41" s="33"/>
     </row>
@@ -5829,11 +5842,11 @@
         <v>102</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>28</v>
@@ -5842,15 +5855,15 @@
         <v>39</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J42" s="34"/>
       <c r="K42" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L42" s="34"/>
       <c r="M42" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N42" s="34"/>
       <c r="O42" s="33"/>
@@ -5862,11 +5875,11 @@
       <c r="B43" s="97"/>
       <c r="C43" s="97"/>
       <c r="D43" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E43" s="28"/>
       <c r="F43" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G43" s="22" t="s">
         <v>28</v>
@@ -5875,15 +5888,15 @@
         <v>39</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J43" s="34"/>
       <c r="K43" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L43" s="34"/>
       <c r="M43" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N43" s="34"/>
       <c r="O43" s="33"/>
@@ -5897,11 +5910,11 @@
         <v>107</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>28</v>
@@ -5910,15 +5923,15 @@
         <v>39</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J44" s="34"/>
       <c r="K44" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N44" s="34"/>
       <c r="O44" s="33"/>
@@ -5936,7 +5949,7 @@
       </c>
       <c r="E45" s="28"/>
       <c r="F45" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G45" s="22" t="s">
         <v>28</v>
@@ -5945,15 +5958,15 @@
         <v>39</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J45" s="34"/>
       <c r="K45" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N45" s="34"/>
       <c r="O45" s="33"/>
@@ -5969,7 +5982,7 @@
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G46" s="22" t="s">
         <v>28</v>
@@ -5978,15 +5991,15 @@
         <v>39</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J46" s="34"/>
       <c r="K46" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L46" s="34"/>
       <c r="M46" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N46" s="34"/>
       <c r="O46" s="33"/>
@@ -6002,7 +6015,7 @@
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G47" s="22" t="s">
         <v>28</v>
@@ -6011,15 +6024,15 @@
         <v>39</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J47" s="34"/>
       <c r="K47" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N47" s="34"/>
       <c r="O47" s="33"/>
@@ -6079,7 +6092,7 @@
         <v>132</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G50" s="22" t="s">
         <v>28</v>
@@ -6094,13 +6107,13 @@
         <v>38</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L50" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M50" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N50" s="34"/>
       <c r="O50" s="33"/>
@@ -6120,7 +6133,7 @@
         <v>204</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G51" s="22" t="s">
         <v>28</v>
@@ -6135,13 +6148,13 @@
         <v>38</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L51" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M51" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N51" s="34"/>
       <c r="O51" s="33"/>
@@ -6159,7 +6172,7 @@
         <v>203</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G52" s="22" t="s">
         <v>28</v>
@@ -6174,13 +6187,13 @@
         <v>38</v>
       </c>
       <c r="K52" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L52" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M52" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N52" s="34"/>
       <c r="O52" s="33"/>
@@ -6200,7 +6213,7 @@
         <v>206</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G53" s="22" t="s">
         <v>28</v>
@@ -6215,13 +6228,13 @@
         <v>38</v>
       </c>
       <c r="K53" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L53" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M53" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N53" s="34"/>
       <c r="O53" s="33"/>
@@ -6241,7 +6254,7 @@
         <v>208</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G54" s="22" t="s">
         <v>28</v>
@@ -6256,13 +6269,13 @@
         <v>38</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L54" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M54" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N54" s="34"/>
       <c r="O54" s="33"/>
@@ -6282,7 +6295,7 @@
         <v>209</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G55" s="22" t="s">
         <v>28</v>
@@ -6297,13 +6310,13 @@
         <v>38</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L55" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M55" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N55" s="34"/>
       <c r="O55" s="33"/>
@@ -6322,22 +6335,22 @@
         <v>17</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H56" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="I56" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="I56" s="22" t="s">
-        <v>239</v>
-      </c>
       <c r="J56" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K56" s="23" t="s">
         <v>30</v>
@@ -6347,7 +6360,7 @@
       </c>
       <c r="M56" s="34"/>
       <c r="N56" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O56" s="33"/>
       <c r="P56" s="33"/>
@@ -6361,10 +6374,10 @@
         <v>134</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>28</v>
@@ -6398,10 +6411,10 @@
         <v>14</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F58" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>28</v>
@@ -6410,13 +6423,13 @@
         <v>123</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J58" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="K58" s="23" t="s">
         <v>243</v>
-      </c>
-      <c r="K58" s="23" t="s">
-        <v>244</v>
       </c>
       <c r="L58" s="22" t="s">
         <v>24</v>
@@ -6438,7 +6451,7 @@
         <v>138</v>
       </c>
       <c r="F59" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G59" s="22" t="s">
         <v>28</v>
@@ -6451,7 +6464,7 @@
       </c>
       <c r="J59" s="34"/>
       <c r="K59" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L59" s="22" t="s">
         <v>24</v>
@@ -6475,7 +6488,7 @@
         <v>142</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G60" s="22" t="s">
         <v>28</v>
@@ -6484,7 +6497,7 @@
         <v>123</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J60" s="22" t="s">
         <v>41</v>
@@ -6509,10 +6522,10 @@
         <v>145</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G61" s="22" t="s">
         <v>28</v>
@@ -6545,25 +6558,25 @@
         <v>9</v>
       </c>
       <c r="D62" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E62" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="E62" s="28" t="s">
+      <c r="F62" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="F62" s="22" t="s">
+      <c r="G62" s="22" t="s">
         <v>230</v>
-      </c>
-      <c r="G62" s="22" t="s">
-        <v>231</v>
       </c>
       <c r="H62" s="22" t="s">
         <v>35</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J62" s="71" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K62" s="23" t="s">
         <v>30</v>
@@ -6573,10 +6586,10 @@
       </c>
       <c r="M62" s="34"/>
       <c r="N62" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O62" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P62" s="33"/>
       <c r="Q62" s="33"/>
@@ -6586,13 +6599,13 @@
       <c r="B63" s="94"/>
       <c r="C63" s="94"/>
       <c r="D63" s="34" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F63" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G63" s="22" t="s">
         <v>28</v>
@@ -6601,7 +6614,7 @@
         <v>39</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J63" s="22" t="s">
         <v>11</v>
@@ -6613,7 +6626,7 @@
         <v>24</v>
       </c>
       <c r="M63" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N63" s="34"/>
       <c r="O63" s="33"/>
@@ -6625,13 +6638,13 @@
       <c r="B64" s="94"/>
       <c r="C64" s="94"/>
       <c r="D64" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E64" s="27" t="s">
         <v>210</v>
       </c>
       <c r="F64" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G64" s="22" t="s">
         <v>28</v>
@@ -6640,19 +6653,19 @@
         <v>39</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J64" s="22" t="s">
         <v>11</v>
       </c>
       <c r="K64" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L64" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M64" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N64" s="34"/>
       <c r="O64" s="33"/>
@@ -6766,10 +6779,10 @@
         <v>193</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F70" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G70" s="22" t="s">
         <v>28</v>
@@ -6778,19 +6791,19 @@
         <v>123</v>
       </c>
       <c r="I70" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J70" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="K70" s="23" t="s">
         <v>247</v>
-      </c>
-      <c r="K70" s="23" t="s">
-        <v>248</v>
       </c>
       <c r="L70" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N70" s="34"/>
       <c r="O70" s="33"/>
@@ -6805,10 +6818,10 @@
         <v>193</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F71" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G71" s="22" t="s">
         <v>28</v>
@@ -6817,19 +6830,19 @@
         <v>39</v>
       </c>
       <c r="I71" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="J71" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="J71" s="14" t="s">
+      <c r="K71" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="K71" s="23" t="s">
-        <v>252</v>
       </c>
       <c r="L71" s="22" t="s">
         <v>24</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N71" s="34"/>
       <c r="O71" s="33"/>
@@ -7100,7 +7113,7 @@
     <mergeCell ref="C58:C59"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J62" r:id="rId1"/>
+    <hyperlink ref="J62" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -7108,7 +7121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -7159,16 +7172,16 @@
         <v>22</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -7206,7 +7219,7 @@
       </c>
       <c r="M2" s="34"/>
       <c r="N2" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
@@ -7216,11 +7229,11 @@
       <c r="B3" s="102"/>
       <c r="C3" s="103"/>
       <c r="D3" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>28</v>
@@ -7236,7 +7249,7 @@
       </c>
       <c r="M3" s="34"/>
       <c r="N3" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
@@ -7246,11 +7259,11 @@
       <c r="B4" s="102"/>
       <c r="C4" s="103"/>
       <c r="D4" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E4" s="37"/>
       <c r="F4" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>28</v>
@@ -7266,7 +7279,7 @@
       </c>
       <c r="M4" s="34"/>
       <c r="N4" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
@@ -7276,11 +7289,11 @@
       <c r="B5" s="105"/>
       <c r="C5" s="106"/>
       <c r="D5" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>28</v>
@@ -7296,7 +7309,7 @@
       </c>
       <c r="M5" s="34"/>
       <c r="N5" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O5" s="48"/>
       <c r="P5" s="48"/>
@@ -7309,7 +7322,7 @@
       <c r="C6" s="94"/>
       <c r="D6" s="94"/>
       <c r="E6" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -7331,7 +7344,7 @@
       <c r="C7" s="94"/>
       <c r="D7" s="94"/>
       <c r="E7" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -7386,17 +7399,17 @@
       <c r="J9" s="34"/>
       <c r="K9" s="27"/>
       <c r="L9" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N9" s="34"/>
       <c r="O9" s="54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P9" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -7407,7 +7420,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
@@ -7416,17 +7429,17 @@
       <c r="J10" s="34"/>
       <c r="K10" s="27"/>
       <c r="L10" s="50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N10" s="34"/>
       <c r="O10" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P10" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -7435,7 +7448,7 @@
       <c r="C11" s="94"/>
       <c r="D11" s="94"/>
       <c r="E11" s="29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
@@ -7444,17 +7457,17 @@
       <c r="J11" s="34"/>
       <c r="K11" s="27"/>
       <c r="L11" s="50" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N11" s="34"/>
       <c r="O11" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P11" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -7463,7 +7476,7 @@
       <c r="C12" s="94"/>
       <c r="D12" s="94"/>
       <c r="E12" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
@@ -7472,17 +7485,17 @@
       <c r="J12" s="34"/>
       <c r="K12" s="27"/>
       <c r="L12" s="50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N12" s="34"/>
       <c r="O12" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P12" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -7491,7 +7504,7 @@
       <c r="C13" s="94"/>
       <c r="D13" s="94"/>
       <c r="E13" s="29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -7500,17 +7513,17 @@
       <c r="J13" s="34"/>
       <c r="K13" s="27"/>
       <c r="L13" s="50" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P13" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -7519,7 +7532,7 @@
       <c r="C14" s="94"/>
       <c r="D14" s="94"/>
       <c r="E14" s="29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
@@ -7528,17 +7541,17 @@
       <c r="J14" s="34"/>
       <c r="K14" s="27"/>
       <c r="L14" s="50" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N14" s="34"/>
       <c r="O14" s="54" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P14" s="55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -7549,7 +7562,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
@@ -7558,10 +7571,10 @@
       <c r="J15" s="34"/>
       <c r="K15" s="27"/>
       <c r="L15" s="50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N15" s="34"/>
     </row>
@@ -7571,7 +7584,7 @@
       <c r="C16" s="94"/>
       <c r="D16" s="94"/>
       <c r="E16" s="29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
@@ -7580,10 +7593,10 @@
       <c r="J16" s="34"/>
       <c r="K16" s="27"/>
       <c r="L16" s="50" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N16" s="34"/>
     </row>
@@ -7593,7 +7606,7 @@
       <c r="C17" s="94"/>
       <c r="D17" s="94"/>
       <c r="E17" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
@@ -7602,10 +7615,10 @@
       <c r="J17" s="34"/>
       <c r="K17" s="27"/>
       <c r="L17" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N17" s="34"/>
     </row>
@@ -7624,10 +7637,10 @@
       <c r="J18" s="34"/>
       <c r="K18" s="27"/>
       <c r="L18" s="50" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N18" s="34"/>
     </row>
@@ -7650,10 +7663,10 @@
       <c r="J19" s="34"/>
       <c r="K19" s="27"/>
       <c r="L19" s="50" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N19" s="34"/>
     </row>
@@ -7676,10 +7689,10 @@
       <c r="J20" s="34"/>
       <c r="K20" s="27"/>
       <c r="L20" s="50" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N20" s="34"/>
     </row>
@@ -7737,7 +7750,7 @@
       <c r="K23" s="27"/>
       <c r="L23" s="22"/>
       <c r="M23" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N23" s="34"/>
     </row>
@@ -7757,7 +7770,7 @@
       <c r="K24" s="27"/>
       <c r="L24" s="22"/>
       <c r="M24" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N24" s="34"/>
     </row>
@@ -7777,7 +7790,7 @@
       <c r="K25" s="27"/>
       <c r="L25" s="22"/>
       <c r="M25" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N25" s="34"/>
     </row>
@@ -7787,7 +7800,7 @@
       <c r="C26" s="97"/>
       <c r="D26" s="97"/>
       <c r="E26" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
@@ -7797,7 +7810,7 @@
       <c r="K26" s="27"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N26" s="34"/>
     </row>
@@ -7807,7 +7820,7 @@
       <c r="C27" s="97"/>
       <c r="D27" s="97"/>
       <c r="E27" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
@@ -7817,7 +7830,7 @@
       <c r="K27" s="27"/>
       <c r="L27" s="22"/>
       <c r="M27" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N27" s="34"/>
     </row>
@@ -7827,7 +7840,7 @@
       <c r="C28" s="97"/>
       <c r="D28" s="97"/>
       <c r="E28" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
@@ -7837,7 +7850,7 @@
       <c r="K28" s="27"/>
       <c r="L28" s="22"/>
       <c r="M28" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N28" s="34"/>
     </row>
@@ -7851,7 +7864,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -7869,7 +7882,7 @@
       <c r="C30" s="97"/>
       <c r="D30" s="97"/>
       <c r="E30" s="29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -7887,7 +7900,7 @@
       <c r="C31" s="97"/>
       <c r="D31" s="97"/>
       <c r="E31" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -7906,10 +7919,10 @@
         <v>21</v>
       </c>
       <c r="D32" s="97" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E32" s="53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -7927,7 +7940,7 @@
       <c r="C33" s="108"/>
       <c r="D33" s="97"/>
       <c r="E33" s="53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
@@ -7945,7 +7958,7 @@
       <c r="C34" s="108"/>
       <c r="D34" s="97"/>
       <c r="E34" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -7963,7 +7976,7 @@
       <c r="C35" s="108"/>
       <c r="D35" s="97"/>
       <c r="E35" s="53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
@@ -7981,7 +7994,7 @@
       <c r="C36" s="108"/>
       <c r="D36" s="97"/>
       <c r="E36" s="53" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -7999,7 +8012,7 @@
       <c r="C37" s="108"/>
       <c r="D37" s="97"/>
       <c r="E37" s="53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -8016,10 +8029,10 @@
       <c r="B38" s="94"/>
       <c r="C38" s="108"/>
       <c r="D38" s="97" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E38" s="53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
@@ -8037,7 +8050,7 @@
       <c r="C39" s="108"/>
       <c r="D39" s="97"/>
       <c r="E39" s="53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
@@ -8055,7 +8068,7 @@
       <c r="C40" s="108"/>
       <c r="D40" s="97"/>
       <c r="E40" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
@@ -8073,7 +8086,7 @@
       <c r="C41" s="109"/>
       <c r="D41" s="97"/>
       <c r="E41" s="53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
@@ -8094,7 +8107,7 @@
         <v>102</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="22"/>
@@ -8105,7 +8118,7 @@
       <c r="K42" s="27"/>
       <c r="L42" s="34"/>
       <c r="M42" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N42" s="34"/>
     </row>
@@ -8114,7 +8127,7 @@
       <c r="B43" s="97"/>
       <c r="C43" s="97"/>
       <c r="D43" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="22"/>
@@ -8125,7 +8138,7 @@
       <c r="K43" s="27"/>
       <c r="L43" s="34"/>
       <c r="M43" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N43" s="34"/>
     </row>
@@ -8136,7 +8149,7 @@
         <v>107</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="22"/>
@@ -8147,7 +8160,7 @@
       <c r="K44" s="27"/>
       <c r="L44" s="34"/>
       <c r="M44" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N44" s="34"/>
     </row>
@@ -8169,7 +8182,7 @@
       <c r="K45" s="27"/>
       <c r="L45" s="34"/>
       <c r="M45" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N45" s="34"/>
     </row>
@@ -8189,7 +8202,7 @@
       <c r="K46" s="27"/>
       <c r="L46" s="34"/>
       <c r="M46" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N46" s="34"/>
     </row>
@@ -8209,7 +8222,7 @@
       <c r="K47" s="27"/>
       <c r="L47" s="34"/>
       <c r="M47" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N47" s="34"/>
     </row>
@@ -8241,7 +8254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -8302,21 +8315,21 @@
         <v>22</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N1" s="40" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
@@ -8347,7 +8360,7 @@
       </c>
       <c r="M2" s="34"/>
       <c r="N2" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
@@ -8357,24 +8370,24 @@
       <c r="B3" s="94"/>
       <c r="C3" s="94"/>
       <c r="D3" s="22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>182</v>
       </c>
       <c r="G3" s="57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="34"/>
@@ -8387,22 +8400,22 @@
       <c r="B4" s="94"/>
       <c r="C4" s="94"/>
       <c r="D4" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="23" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="34"/>
@@ -8415,11 +8428,11 @@
       <c r="B5" s="94"/>
       <c r="C5" s="94"/>
       <c r="D5" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
@@ -8437,7 +8450,7 @@
       <c r="B6" s="94"/>
       <c r="C6" s="94"/>
       <c r="D6" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="22" t="s">
@@ -8457,7 +8470,7 @@
       </c>
       <c r="M6" s="34"/>
       <c r="N6" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O6" s="48"/>
       <c r="P6" s="48"/>
@@ -8467,7 +8480,7 @@
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
       <c r="D7" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="22" t="s">
@@ -8487,7 +8500,7 @@
       </c>
       <c r="M7" s="34"/>
       <c r="N7" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O7" s="48"/>
       <c r="P7" s="48"/>
@@ -8515,7 +8528,7 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="22" t="s">
@@ -8535,7 +8548,7 @@
       </c>
       <c r="M9" s="34"/>
       <c r="N9" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O9" s="48"/>
       <c r="P9" s="48"/>
@@ -8548,7 +8561,7 @@
       <c r="C10" s="94"/>
       <c r="D10" s="94"/>
       <c r="E10" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
@@ -8570,7 +8583,7 @@
       <c r="C11" s="94"/>
       <c r="D11" s="94"/>
       <c r="E11" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
@@ -8615,22 +8628,22 @@
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13" s="26"/>
       <c r="F13" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="30"/>
       <c r="J13" s="22"/>
       <c r="K13" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L13" s="22"/>
       <c r="M13" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N13" s="36"/>
       <c r="O13" s="27"/>
@@ -8644,22 +8657,22 @@
         <v>18</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="30"/>
       <c r="J14" s="22"/>
       <c r="K14" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N14" s="36"/>
       <c r="O14" s="27"/>
@@ -8671,22 +8684,22 @@
       <c r="B15" s="94"/>
       <c r="C15" s="94"/>
       <c r="D15" s="26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="I15" s="30"/>
       <c r="J15" s="22"/>
       <c r="K15" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L15" s="22"/>
       <c r="M15" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N15" s="36"/>
       <c r="O15" s="27"/>
@@ -8698,22 +8711,22 @@
       <c r="B16" s="94"/>
       <c r="C16" s="94"/>
       <c r="D16" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="30"/>
       <c r="J16" s="22"/>
       <c r="K16" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N16" s="36"/>
       <c r="O16" s="27"/>
@@ -8725,22 +8738,22 @@
       <c r="B17" s="94"/>
       <c r="C17" s="94"/>
       <c r="D17" s="26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="30"/>
       <c r="J17" s="22"/>
       <c r="K17" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L17" s="22"/>
       <c r="M17" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N17" s="36"/>
       <c r="O17" s="27"/>
@@ -8751,22 +8764,22 @@
       <c r="B18" s="94"/>
       <c r="C18" s="94"/>
       <c r="D18" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E18" s="26"/>
       <c r="F18" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
       <c r="I18" s="30"/>
       <c r="J18" s="22"/>
       <c r="K18" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N18" s="36"/>
       <c r="O18" s="27"/>
@@ -8779,22 +8792,22 @@
         <v>19</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E19" s="26"/>
       <c r="F19" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="30"/>
       <c r="J19" s="22"/>
       <c r="K19" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L19" s="22"/>
       <c r="M19" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N19" s="36"/>
       <c r="O19" s="27"/>
@@ -8805,22 +8818,22 @@
       <c r="B20" s="94"/>
       <c r="C20" s="94"/>
       <c r="D20" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E20" s="26"/>
       <c r="F20" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="56"/>
       <c r="J20" s="22"/>
       <c r="K20" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L20" s="22"/>
       <c r="M20" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N20" s="36"/>
       <c r="O20" s="27"/>
@@ -8831,22 +8844,22 @@
       <c r="B21" s="94"/>
       <c r="C21" s="94"/>
       <c r="D21" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E21" s="26"/>
       <c r="F21" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="56"/>
       <c r="J21" s="22"/>
       <c r="K21" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N21" s="36"/>
       <c r="O21" s="27"/>
@@ -8857,22 +8870,22 @@
       <c r="B22" s="94"/>
       <c r="C22" s="94"/>
       <c r="D22" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
       <c r="I22" s="56"/>
       <c r="J22" s="22"/>
       <c r="K22" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L22" s="22"/>
       <c r="M22" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="27"/>
@@ -8883,22 +8896,22 @@
       <c r="B23" s="94"/>
       <c r="C23" s="94"/>
       <c r="D23" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="56"/>
       <c r="J23" s="22"/>
       <c r="K23" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L23" s="22"/>
       <c r="M23" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N23" s="36"/>
       <c r="O23" s="27"/>
@@ -8909,22 +8922,22 @@
       <c r="B24" s="94"/>
       <c r="C24" s="94"/>
       <c r="D24" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E24" s="26"/>
       <c r="F24" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
       <c r="I24" s="30"/>
       <c r="J24" s="22"/>
       <c r="K24" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N24" s="36"/>
       <c r="O24" s="27"/>
@@ -8935,22 +8948,22 @@
       <c r="B25" s="94"/>
       <c r="C25" s="94"/>
       <c r="D25" s="26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="30"/>
       <c r="J25" s="22"/>
       <c r="K25" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L25" s="22"/>
       <c r="M25" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N25" s="36"/>
       <c r="O25" s="27"/>
@@ -8961,22 +8974,22 @@
       <c r="B26" s="94"/>
       <c r="C26" s="94"/>
       <c r="D26" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="56"/>
       <c r="J26" s="22"/>
       <c r="K26" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L26" s="22"/>
       <c r="M26" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N26" s="36"/>
       <c r="O26" s="27"/>
@@ -8987,22 +9000,22 @@
       <c r="B27" s="94"/>
       <c r="C27" s="94"/>
       <c r="D27" s="26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E27" s="26"/>
       <c r="F27" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="56"/>
       <c r="J27" s="22"/>
       <c r="K27" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L27" s="22"/>
       <c r="M27" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N27" s="36"/>
       <c r="O27" s="27"/>
@@ -9013,22 +9026,22 @@
       <c r="B28" s="94"/>
       <c r="C28" s="94"/>
       <c r="D28" s="42" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
       <c r="I28" s="30"/>
       <c r="J28" s="22"/>
       <c r="K28" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L28" s="22"/>
       <c r="M28" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N28" s="36"/>
       <c r="O28" s="27"/>
@@ -9043,29 +9056,29 @@
         <v>71</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E29" s="65"/>
       <c r="F29" s="66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G29" s="66"/>
       <c r="H29" s="66"/>
       <c r="I29" s="67"/>
       <c r="J29" s="66"/>
       <c r="K29" s="68" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L29" s="69"/>
       <c r="M29" s="70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N29" s="70"/>
       <c r="O29" s="66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P29" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -9077,11 +9090,11 @@
         <v>74</v>
       </c>
       <c r="D30" s="65" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E30" s="65"/>
       <c r="F30" s="66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G30" s="66"/>
       <c r="H30" s="66"/>
@@ -9092,10 +9105,10 @@
       <c r="M30" s="66"/>
       <c r="N30" s="70"/>
       <c r="O30" s="69" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P30" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -9111,7 +9124,7 @@
       </c>
       <c r="E31" s="65"/>
       <c r="F31" s="66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G31" s="66"/>
       <c r="H31" s="66"/>
@@ -9122,10 +9135,10 @@
       <c r="M31" s="66"/>
       <c r="N31" s="70"/>
       <c r="O31" s="69" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P31" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -9137,7 +9150,7 @@
       </c>
       <c r="E32" s="65"/>
       <c r="F32" s="66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G32" s="66"/>
       <c r="H32" s="66"/>
@@ -9148,10 +9161,10 @@
       <c r="M32" s="66"/>
       <c r="N32" s="70"/>
       <c r="O32" s="69" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P32" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -9163,22 +9176,22 @@
         <v>82</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
       <c r="I33" s="56"/>
       <c r="J33" s="22"/>
       <c r="K33" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L33" s="22"/>
       <c r="M33" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N33" s="59"/>
       <c r="O33" s="48"/>
@@ -9189,22 +9202,22 @@
       <c r="B34" s="94"/>
       <c r="C34" s="94"/>
       <c r="D34" s="60" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E34" s="28"/>
       <c r="F34" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
       <c r="I34" s="56"/>
       <c r="J34" s="22"/>
       <c r="K34" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L34" s="22"/>
       <c r="M34" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N34" s="59"/>
       <c r="O34" s="48"/>
@@ -9215,22 +9228,22 @@
       <c r="B35" s="94"/>
       <c r="C35" s="94"/>
       <c r="D35" s="60" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E35" s="28"/>
       <c r="F35" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="56"/>
       <c r="J35" s="22"/>
       <c r="K35" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L35" s="22"/>
       <c r="M35" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N35" s="59"/>
       <c r="O35" s="48"/>
@@ -9241,22 +9254,22 @@
       <c r="B36" s="94"/>
       <c r="C36" s="94"/>
       <c r="D36" s="60" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E36" s="28"/>
       <c r="F36" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
       <c r="I36" s="56"/>
       <c r="J36" s="22"/>
       <c r="K36" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L36" s="22"/>
       <c r="M36" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N36" s="59"/>
       <c r="O36" s="48"/>
@@ -9267,22 +9280,22 @@
       <c r="B37" s="94"/>
       <c r="C37" s="94"/>
       <c r="D37" s="60" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
       <c r="I37" s="56"/>
       <c r="J37" s="22"/>
       <c r="K37" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L37" s="22"/>
       <c r="M37" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N37" s="59"/>
       <c r="O37" s="48"/>
@@ -9293,22 +9306,22 @@
       <c r="B38" s="94"/>
       <c r="C38" s="94"/>
       <c r="D38" s="60" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
       <c r="I38" s="56"/>
       <c r="J38" s="22"/>
       <c r="K38" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L38" s="22"/>
       <c r="M38" s="59" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N38" s="59"/>
       <c r="O38" s="48"/>
@@ -9323,22 +9336,22 @@
         <v>20</v>
       </c>
       <c r="D39" s="61" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
       <c r="I39" s="56"/>
       <c r="J39" s="22"/>
       <c r="K39" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L39" s="22"/>
       <c r="M39" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N39" s="59"/>
       <c r="O39" s="48"/>
@@ -9349,22 +9362,22 @@
       <c r="B40" s="109"/>
       <c r="C40" s="109"/>
       <c r="D40" s="28" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
       <c r="I40" s="56"/>
       <c r="J40" s="22"/>
       <c r="K40" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L40" s="22"/>
       <c r="M40" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N40" s="59"/>
       <c r="O40" s="48"/>
@@ -9423,22 +9436,22 @@
         <v>102</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E43" s="28"/>
       <c r="F43" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
       <c r="I43" s="56"/>
       <c r="J43" s="22"/>
       <c r="K43" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L43" s="22"/>
       <c r="M43" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N43" s="34"/>
       <c r="O43" s="48"/>
@@ -9449,22 +9462,22 @@
       <c r="B44" s="97"/>
       <c r="C44" s="97"/>
       <c r="D44" s="28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
       <c r="I44" s="56"/>
       <c r="J44" s="22"/>
       <c r="K44" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L44" s="22"/>
       <c r="M44" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N44" s="34"/>
       <c r="O44" s="48"/>
@@ -9475,22 +9488,22 @@
       <c r="B45" s="97"/>
       <c r="C45" s="97"/>
       <c r="D45" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E45" s="28"/>
       <c r="F45" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
       <c r="I45" s="56"/>
       <c r="J45" s="22"/>
       <c r="K45" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L45" s="22"/>
       <c r="M45" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N45" s="34"/>
       <c r="O45" s="48"/>
@@ -9501,22 +9514,22 @@
       <c r="B46" s="97"/>
       <c r="C46" s="97"/>
       <c r="D46" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
       <c r="I46" s="56"/>
       <c r="J46" s="22"/>
       <c r="K46" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L46" s="22"/>
       <c r="M46" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N46" s="34"/>
       <c r="O46" s="48"/>
@@ -9529,22 +9542,22 @@
         <v>107</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E47" s="28"/>
       <c r="F47" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
       <c r="I47" s="56"/>
       <c r="J47" s="22"/>
       <c r="K47" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L47" s="22"/>
       <c r="M47" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N47" s="34"/>
       <c r="O47" s="48"/>
@@ -9555,22 +9568,22 @@
       <c r="B48" s="97"/>
       <c r="C48" s="97"/>
       <c r="D48" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E48" s="28"/>
       <c r="F48" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
       <c r="I48" s="56"/>
       <c r="J48" s="22"/>
       <c r="K48" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L48" s="22"/>
       <c r="M48" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N48" s="34"/>
       <c r="O48" s="48"/>
@@ -9581,22 +9594,22 @@
       <c r="B49" s="97"/>
       <c r="C49" s="97"/>
       <c r="D49" s="42" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E49" s="28"/>
       <c r="F49" s="22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
       <c r="I49" s="56"/>
       <c r="J49" s="22"/>
       <c r="K49" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L49" s="22"/>
       <c r="M49" s="48" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N49" s="34"/>
       <c r="O49" s="48"/>
@@ -9826,22 +9839,22 @@
       </c>
       <c r="D67" s="26"/>
       <c r="E67" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F67" s="22"/>
       <c r="G67" s="22"/>
       <c r="H67" s="56"/>
       <c r="I67" s="22"/>
       <c r="J67" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K67" s="22"/>
       <c r="L67" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M67" s="36"/>
       <c r="N67" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
@@ -9850,22 +9863,22 @@
       </c>
       <c r="D68" s="26"/>
       <c r="E68" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F68" s="22"/>
       <c r="G68" s="22"/>
       <c r="H68" s="56"/>
       <c r="I68" s="22"/>
       <c r="J68" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K68" s="22"/>
       <c r="L68" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M68" s="36"/>
       <c r="N68" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
@@ -9874,22 +9887,22 @@
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F69" s="22"/>
       <c r="G69" s="22"/>
       <c r="H69" s="56"/>
       <c r="I69" s="22"/>
       <c r="J69" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K69" s="22"/>
       <c r="L69" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M69" s="36"/>
       <c r="N69" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
@@ -9898,22 +9911,22 @@
       </c>
       <c r="D70" s="26"/>
       <c r="E70" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F70" s="22"/>
       <c r="G70" s="22"/>
       <c r="H70" s="56"/>
       <c r="I70" s="22"/>
       <c r="J70" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K70" s="22"/>
       <c r="L70" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M70" s="36"/>
       <c r="N70" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
@@ -9922,22 +9935,22 @@
       </c>
       <c r="D71" s="26"/>
       <c r="E71" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F71" s="22"/>
       <c r="G71" s="22"/>
       <c r="H71" s="56"/>
       <c r="I71" s="22"/>
       <c r="J71" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K71" s="22"/>
       <c r="L71" s="34" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M71" s="36"/>
       <c r="N71" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
@@ -10321,7 +10334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">

</xml_diff>